<commit_message>
Cambio en digito verificador el rut terminado en 9
</commit_message>
<xml_diff>
--- a/backend/src/data/usuarios.xlsx
+++ b/backend/src/data/usuarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Electivos-ISW\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{353B975D-45E4-41E3-B6F5-C2D5A527FC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5C1828-601E-48FB-8EE8-FB40AC36614F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4E5DF0B-E93F-4392-91DE-3A1947C02294}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C4E5DF0B-E93F-4392-91DE-3A1947C02294}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>juan.perez@profesor.cl</t>
   </si>
   <si>
-    <t>12345678-9</t>
-  </si>
-  <si>
     <t>PROFESOR</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>22333444-5</t>
+  </si>
+  <si>
+    <t>12345678-5</t>
   </si>
 </sst>
 </file>
@@ -538,18 +538,18 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -577,7 +577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -585,80 +585,80 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicion de carrera a tabla user, arreglo de cambios en backend y frontend
</commit_message>
<xml_diff>
--- a/backend/src/data/usuarios.xlsx
+++ b/backend/src/data/usuarios.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Electivos-ISW\backend\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juanp\Desktop\Programitas\Electivos-ISW\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5C1828-601E-48FB-8EE8-FB40AC36614F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C4E5DF0B-E93F-4392-91DE-3A1947C02294}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Nombre</t>
   </si>
@@ -120,13 +119,25 @@
   </si>
   <si>
     <t>12345678-5</t>
+  </si>
+  <si>
+    <t>Carrera</t>
+  </si>
+  <si>
+    <t>Ingeniería Civil en Informática</t>
+  </si>
+  <si>
+    <t>Ingeniería de Ejecución en Computación</t>
+  </si>
+  <si>
+    <t>Ingeniería Civil Industrial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,22 +545,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72ED7444-1025-4106-9EEB-A5A4F43B6ABD}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.125" customWidth="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
+    <col min="4" max="4" width="22.25" customWidth="1"/>
+    <col min="5" max="5" width="35.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,8 +574,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -576,8 +591,9 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -590,8 +606,9 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -604,8 +621,9 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -618,8 +636,11 @@
       <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -632,8 +653,11 @@
       <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -646,8 +670,11 @@
       <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -659,6 +686,9 @@
       </c>
       <c r="D8" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregando periodo y validaciones de jefe de carrera
</commit_message>
<xml_diff>
--- a/backend/src/data/usuarios.xlsx
+++ b/backend/src/data/usuarios.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Nombre</t>
   </si>
@@ -131,13 +131,22 @@
   </si>
   <si>
     <t>Ingeniería Civil Industrial</t>
+  </si>
+  <si>
+    <t>Parra</t>
+  </si>
+  <si>
+    <t>jefe.parra@universidad.cl</t>
+  </si>
+  <si>
+    <t>22222222-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +174,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -174,7 +191,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,11 +214,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
@@ -212,8 +241,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -591,7 +627,9 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1">
       <c r="A3" s="2" t="s">
@@ -691,8 +729,28 @@
         <v>29</v>
       </c>
     </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1">
+      <c r="A9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Creacion sistema de correos, gestion de restricciones para los user en etapas de inscripcion o fuera de estas
</commit_message>
<xml_diff>
--- a/backend/src/data/usuarios.xlsx
+++ b/backend/src/data/usuarios.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Nombre</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>22222222-2</t>
+  </si>
+  <si>
+    <t>Juan Pablo</t>
+  </si>
+  <si>
+    <t>juan.villagra2201@alumnos.ubiobio.cl</t>
+  </si>
+  <si>
+    <t>20680787-3</t>
   </si>
 </sst>
 </file>
@@ -230,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
@@ -247,6 +256,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -582,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -746,11 +756,29 @@
         <v>30</v>
       </c>
     </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ruts con digito verificador valido
</commit_message>
<xml_diff>
--- a/backend/src/data/usuarios.xlsx
+++ b/backend/src/data/usuarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juanp\Desktop\Programitas\Electivos-ISW\backend\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Electivos-ISW\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B7FBA0-5070-4255-8755-3B5DC4AFA5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -76,18 +66,12 @@
     <t>maria.silva@profesor.cl</t>
   </si>
   <si>
-    <t>9876543-2</t>
-  </si>
-  <si>
     <t>Carlos Díaz</t>
   </si>
   <si>
     <t>carlos.diaz@alumno.cl</t>
   </si>
   <si>
-    <t>20555666-K</t>
-  </si>
-  <si>
     <t>ALUMNO</t>
   </si>
   <si>
@@ -97,27 +81,18 @@
     <t>ana.torres@alumno.cl</t>
   </si>
   <si>
-    <t>21123456-7</t>
-  </si>
-  <si>
     <t>Fabian Test</t>
   </si>
   <si>
     <t>fabian.test@alumno.cl</t>
   </si>
   <si>
-    <t>19999888-0</t>
-  </si>
-  <si>
     <t>Sofia Lagos</t>
   </si>
   <si>
     <t>sofia.lagos@alumno.cl</t>
   </si>
   <si>
-    <t>22333444-5</t>
-  </si>
-  <si>
     <t>12345678-5</t>
   </si>
   <si>
@@ -149,13 +124,28 @@
   </si>
   <si>
     <t>20680787-3</t>
+  </si>
+  <si>
+    <t>9876543-3</t>
+  </si>
+  <si>
+    <t>20555666-4</t>
+  </si>
+  <si>
+    <t>21123456-3</t>
+  </si>
+  <si>
+    <t>19999888-9</t>
+  </si>
+  <si>
+    <t>22333444-K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,7 +240,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -591,23 +581,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34.125" customWidth="1"/>
-    <col min="3" max="3" width="15.125" customWidth="1"/>
-    <col min="4" max="4" width="22.25" customWidth="1"/>
-    <col min="5" max="5" width="35.75" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,10 +611,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -638,10 +628,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -649,14 +639,14 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -664,119 +654,119 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1">
-      <c r="A9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="B10" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1"/>
-    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Guardado temporal antes de merge
</commit_message>
<xml_diff>
--- a/backend/src/data/usuarios.xlsx
+++ b/backend/src/data/usuarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juanp\Desktop\Programitas\Electivos-ISW\backend\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\proyecto isw\Electivos-ISW\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165C0EC4-6840-4ED7-BC2A-B7E93C1BEBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="5952" yWindow="3312" windowWidth="13548" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Nombre</t>
   </si>
@@ -149,13 +139,22 @@
   </si>
   <si>
     <t>20680787-3</t>
+  </si>
+  <si>
+    <t>Carlos Cadiz</t>
+  </si>
+  <si>
+    <t>carloscadiz2805@gmail.com</t>
+  </si>
+  <si>
+    <t>21019653-6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,7 +199,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -234,12 +233,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
@@ -250,13 +258,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -591,23 +605,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34.125" customWidth="1"/>
-    <col min="3" max="3" width="15.125" customWidth="1"/>
-    <col min="4" max="4" width="22.25" customWidth="1"/>
-    <col min="5" max="5" width="35.75" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.21875" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +638,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -641,7 +655,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -656,7 +670,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1">
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -671,7 +685,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -688,7 +702,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1">
+    <row r="6" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -705,7 +719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1">
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -722,7 +736,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -739,7 +753,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1">
+    <row r="9" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
@@ -756,7 +770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
@@ -773,12 +787,30 @@
         <v>29</v>
       </c>
     </row>
+    <row r="11" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1"/>
-    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{D7173165-5C8E-41D6-ADB8-B36605544E9A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DESCARGAR LISTA DE ALUMNOS COMO PDF
</commit_message>
<xml_diff>
--- a/backend/src/data/usuarios.xlsx
+++ b/backend/src/data/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Electivos-ISW\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB83AB8-6F0D-4789-8AD5-25F3DE6224FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4659166B-C2CF-469F-882F-6F5D7944DCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -606,7 +606,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ruts validos para pruebas y 3 ruts invalidos para pruebas
</commit_message>
<xml_diff>
--- a/backend/src/data/usuarios.xlsx
+++ b/backend/src/data/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Electivos-ISW\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4659166B-C2CF-469F-882F-6F5D7944DCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7D7427-DE27-479B-9353-85E7F72382BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
   <si>
     <t>Nombre</t>
   </si>
@@ -66,9 +66,6 @@
     <t>maria.silva@profesor.cl</t>
   </si>
   <si>
-    <t>9876543-2</t>
-  </si>
-  <si>
     <t>Carlos Díaz</t>
   </si>
   <si>
@@ -84,27 +81,18 @@
     <t>ana.torres@alumno.cl</t>
   </si>
   <si>
-    <t>21123456-7</t>
-  </si>
-  <si>
     <t>Fabian Test</t>
   </si>
   <si>
     <t>fabian.test@alumno.cl</t>
   </si>
   <si>
-    <t>19999888-0</t>
-  </si>
-  <si>
     <t>Sofia Lagos</t>
   </si>
   <si>
     <t>sofia.lagos@alumno.cl</t>
   </si>
   <si>
-    <t>22333444-5</t>
-  </si>
-  <si>
     <t>12345678-5</t>
   </si>
   <si>
@@ -148,13 +136,166 @@
   </si>
   <si>
     <t>20555666-4</t>
+  </si>
+  <si>
+    <t>camila.rojas@alumno.cl</t>
+  </si>
+  <si>
+    <t>Ingeniería de Ejecución en Computación e Informática</t>
+  </si>
+  <si>
+    <t>felipe.gonzalez@alumno.cl</t>
+  </si>
+  <si>
+    <t>Derecho</t>
+  </si>
+  <si>
+    <t>andrea.pizarro@alumno.cl</t>
+  </si>
+  <si>
+    <t>Ingeniería Comercial</t>
+  </si>
+  <si>
+    <t>jorge.munoz@universidad.cl</t>
+  </si>
+  <si>
+    <t>16.666.666-K</t>
+  </si>
+  <si>
+    <t>patricia.leiva@profesor.cl</t>
+  </si>
+  <si>
+    <t>17.111.222-2</t>
+  </si>
+  <si>
+    <t>nicolas.vera@alumno.cl</t>
+  </si>
+  <si>
+    <t>23.456.789-6</t>
+  </si>
+  <si>
+    <t>valentina.soto@alumno.cl</t>
+  </si>
+  <si>
+    <t>24.000.001-6</t>
+  </si>
+  <si>
+    <t>roberto.castillo@profesor.cl</t>
+  </si>
+  <si>
+    <t>12.876.543-3</t>
+  </si>
+  <si>
+    <t>esteban.paredes@alumno.cl</t>
+  </si>
+  <si>
+    <t>19.876.543-0</t>
+  </si>
+  <si>
+    <t>lucia.mendez@universidad.cl</t>
+  </si>
+  <si>
+    <t>diego.araya@alumno.cl</t>
+  </si>
+  <si>
+    <t>20.555.666-9</t>
+  </si>
+  <si>
+    <t>Ingenieria Civil en Informática</t>
+  </si>
+  <si>
+    <t>prueba.error.alumno@alumno.cl</t>
+  </si>
+  <si>
+    <t>prueba.error.profesor@profesor.cl</t>
+  </si>
+  <si>
+    <t>prueba.error.jefecarrera@jefe.cl</t>
+  </si>
+  <si>
+    <t>14.200.300-K</t>
+  </si>
+  <si>
+    <t>Ingenieria Comercial</t>
+  </si>
+  <si>
+    <t>21456789-K</t>
+  </si>
+  <si>
+    <t>20999888-2</t>
+  </si>
+  <si>
+    <t>22123456-1</t>
+  </si>
+  <si>
+    <t>15.555.444-4</t>
+  </si>
+  <si>
+    <t>21.005.005-1</t>
+  </si>
+  <si>
+    <t>9876543-3</t>
+  </si>
+  <si>
+    <t>21123456-3</t>
+  </si>
+  <si>
+    <t>19999888-9</t>
+  </si>
+  <si>
+    <t>22333444-k</t>
+  </si>
+  <si>
+    <t>Camila Rojas</t>
+  </si>
+  <si>
+    <t>Felipe Gonzalez</t>
+  </si>
+  <si>
+    <t>Andrea Pizarro</t>
+  </si>
+  <si>
+    <t>Jorge Munoz</t>
+  </si>
+  <si>
+    <t>Patricia Leiva</t>
+  </si>
+  <si>
+    <t>Nicolas Vera</t>
+  </si>
+  <si>
+    <t>Valentina Soto</t>
+  </si>
+  <si>
+    <t>Roberto Castillo</t>
+  </si>
+  <si>
+    <t>Esteban Paredes</t>
+  </si>
+  <si>
+    <t>Lucia Mendez</t>
+  </si>
+  <si>
+    <t>Diego Araya</t>
+  </si>
+  <si>
+    <t>Prueba Error.Alumno</t>
+  </si>
+  <si>
+    <t>Prueba Error.Profesor</t>
+  </si>
+  <si>
+    <t>Prueba Error.Jefecarrera</t>
+  </si>
+  <si>
+    <t>10.555.111-7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +331,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -199,7 +348,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -242,12 +391,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
@@ -266,6 +424,22 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -603,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +792,7 @@
     <col min="5" max="5" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,10 +806,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -649,10 +823,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -660,14 +834,14 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -675,130 +849,369 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="C9" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>29</v>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -806,8 +1219,14 @@
     <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B11" r:id="rId3" xr:uid="{D7173165-5C8E-41D6-ADB8-B36605544E9A}"/>
+    <hyperlink ref="B23" r:id="rId4" xr:uid="{706C9537-2898-4062-9DB8-5DDBA3F44F32}"/>
+    <hyperlink ref="B24" r:id="rId5" xr:uid="{43A0223C-93D5-4180-8681-79E9E66F4386}"/>
+    <hyperlink ref="B25" r:id="rId6" xr:uid="{7CBC1987-F552-4F7E-A63A-C72CE1B5D3B1}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{D407A97C-E0FC-4B26-8450-83AF01C4E472}"/>
+    <hyperlink ref="B6" r:id="rId8" xr:uid="{3E997090-AC10-4512-9E0D-9521BBE07A98}"/>
+    <hyperlink ref="B7" r:id="rId9" xr:uid="{EA1A1D94-F37E-4492-AB8C-89BBC5CC2BB0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios en validacioens y excel
</commit_message>
<xml_diff>
--- a/backend/src/data/usuarios.xlsx
+++ b/backend/src/data/usuarios.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Electivos-ISW\backend\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juanp\Desktop\Programitas\Electivos-ISW\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7D7427-DE27-479B-9353-85E7F72382BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Nombre</t>
   </si>
@@ -81,6 +80,9 @@
     <t>ana.torres@alumno.cl</t>
   </si>
   <si>
+    <t>21123456-7</t>
+  </si>
+  <si>
     <t>Fabian Test</t>
   </si>
   <si>
@@ -93,7 +95,7 @@
     <t>sofia.lagos@alumno.cl</t>
   </si>
   <si>
-    <t>12345678-5</t>
+    <t>22333444-5</t>
   </si>
   <si>
     <t>Carrera</t>
@@ -138,164 +140,20 @@
     <t>20555666-4</t>
   </si>
   <si>
-    <t>camila.rojas@alumno.cl</t>
-  </si>
-  <si>
-    <t>Ingeniería de Ejecución en Computación e Informática</t>
-  </si>
-  <si>
-    <t>felipe.gonzalez@alumno.cl</t>
-  </si>
-  <si>
-    <t>Derecho</t>
-  </si>
-  <si>
-    <t>andrea.pizarro@alumno.cl</t>
-  </si>
-  <si>
-    <t>Ingeniería Comercial</t>
-  </si>
-  <si>
-    <t>jorge.munoz@universidad.cl</t>
-  </si>
-  <si>
-    <t>16.666.666-K</t>
-  </si>
-  <si>
-    <t>patricia.leiva@profesor.cl</t>
-  </si>
-  <si>
-    <t>17.111.222-2</t>
-  </si>
-  <si>
-    <t>nicolas.vera@alumno.cl</t>
-  </si>
-  <si>
-    <t>23.456.789-6</t>
-  </si>
-  <si>
-    <t>valentina.soto@alumno.cl</t>
-  </si>
-  <si>
-    <t>24.000.001-6</t>
-  </si>
-  <si>
-    <t>roberto.castillo@profesor.cl</t>
-  </si>
-  <si>
-    <t>12.876.543-3</t>
-  </si>
-  <si>
-    <t>esteban.paredes@alumno.cl</t>
-  </si>
-  <si>
-    <t>19.876.543-0</t>
-  </si>
-  <si>
-    <t>lucia.mendez@universidad.cl</t>
-  </si>
-  <si>
-    <t>diego.araya@alumno.cl</t>
-  </si>
-  <si>
-    <t>20.555.666-9</t>
-  </si>
-  <si>
-    <t>Ingenieria Civil en Informática</t>
-  </si>
-  <si>
-    <t>prueba.error.alumno@alumno.cl</t>
-  </si>
-  <si>
-    <t>prueba.error.profesor@profesor.cl</t>
-  </si>
-  <si>
-    <t>prueba.error.jefecarrera@jefe.cl</t>
-  </si>
-  <si>
-    <t>14.200.300-K</t>
-  </si>
-  <si>
-    <t>Ingenieria Comercial</t>
-  </si>
-  <si>
-    <t>21456789-K</t>
-  </si>
-  <si>
-    <t>20999888-2</t>
-  </si>
-  <si>
-    <t>22123456-1</t>
-  </si>
-  <si>
-    <t>15.555.444-4</t>
-  </si>
-  <si>
-    <t>21.005.005-1</t>
-  </si>
-  <si>
-    <t>9876543-3</t>
-  </si>
-  <si>
-    <t>21123456-3</t>
-  </si>
-  <si>
-    <t>19999888-9</t>
-  </si>
-  <si>
-    <t>22333444-k</t>
-  </si>
-  <si>
-    <t>Camila Rojas</t>
-  </si>
-  <si>
-    <t>Felipe Gonzalez</t>
-  </si>
-  <si>
-    <t>Andrea Pizarro</t>
-  </si>
-  <si>
-    <t>Jorge Munoz</t>
-  </si>
-  <si>
-    <t>Patricia Leiva</t>
-  </si>
-  <si>
-    <t>Nicolas Vera</t>
-  </si>
-  <si>
-    <t>Valentina Soto</t>
-  </si>
-  <si>
-    <t>Roberto Castillo</t>
-  </si>
-  <si>
-    <t>Esteban Paredes</t>
-  </si>
-  <si>
-    <t>Lucia Mendez</t>
-  </si>
-  <si>
-    <t>Diego Araya</t>
-  </si>
-  <si>
-    <t>Prueba Error.Alumno</t>
-  </si>
-  <si>
-    <t>Prueba Error.Profesor</t>
-  </si>
-  <si>
-    <t>Prueba Error.Jefecarrera</t>
-  </si>
-  <si>
-    <t>10.555.111-7</t>
+    <t>18765432-7</t>
+  </si>
+  <si>
+    <t>7618285-K</t>
+  </si>
+  <si>
+    <t>15789123-5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,14 +189,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -348,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -391,21 +241,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
@@ -424,22 +265,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -776,23 +601,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.125" customWidth="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
+    <col min="4" max="4" width="22.25" customWidth="1"/>
+    <col min="5" max="5" width="35.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,10 +631,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -823,10 +648,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -834,14 +659,14 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -849,14 +674,14 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -864,369 +689,124 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1">
       <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B11" r:id="rId3" xr:uid="{D7173165-5C8E-41D6-ADB8-B36605544E9A}"/>
-    <hyperlink ref="B23" r:id="rId4" xr:uid="{706C9537-2898-4062-9DB8-5DDBA3F44F32}"/>
-    <hyperlink ref="B24" r:id="rId5" xr:uid="{43A0223C-93D5-4180-8681-79E9E66F4386}"/>
-    <hyperlink ref="B25" r:id="rId6" xr:uid="{7CBC1987-F552-4F7E-A63A-C72CE1B5D3B1}"/>
-    <hyperlink ref="B12" r:id="rId7" xr:uid="{D407A97C-E0FC-4B26-8450-83AF01C4E472}"/>
-    <hyperlink ref="B6" r:id="rId8" xr:uid="{3E997090-AC10-4512-9E0D-9521BBE07A98}"/>
-    <hyperlink ref="B7" r:id="rId9" xr:uid="{EA1A1D94-F37E-4492-AB8C-89BBC5CC2BB0}"/>
+    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>